<commit_message>
saving the similarity matrix
</commit_message>
<xml_diff>
--- a/Mappings/Proposal-Catrgories-mapped-to-responses.xlsx
+++ b/Mappings/Proposal-Catrgories-mapped-to-responses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
   </bookViews>
   <sheets>
     <sheet name="ENV (Proposal)" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Coverage w.r.t proposal categories</t>
   </si>
@@ -72,15 +72,6 @@
     <t>Normalised Count/ Density</t>
   </si>
   <si>
-    <t>Uncategorised</t>
-  </si>
-  <si>
-    <t>Absent in the Proposal</t>
-  </si>
-  <si>
-    <t>Occurences</t>
-  </si>
-  <si>
     <t xml:space="preserve">Catogory </t>
   </si>
   <si>
@@ -102,7 +93,19 @@
     <t>Large Parks</t>
   </si>
   <si>
-    <t>Absent in the Proposal/ Uncategorized</t>
+    <t>Category w.r.t proposal categories</t>
+  </si>
+  <si>
+    <t>Response Occurences</t>
+  </si>
+  <si>
+    <t>Uncategorised Responses</t>
+  </si>
+  <si>
+    <t>Uncategorized Responses</t>
+  </si>
+  <si>
+    <t>Category Present in the Proposal</t>
   </si>
 </sst>
 </file>
@@ -309,7 +312,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Occurences</c:v>
+                  <c:v>Response Occurences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -398,6 +401,9 @@
                 <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
@@ -406,6 +412,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,7 +429,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absent in the Proposal</c:v>
+                  <c:v>Category Present in the Proposal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -488,8 +497,38 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -507,7 +546,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Uncategorised</c:v>
+                  <c:v>Uncategorised Responses</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -591,11 +630,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="572682744"/>
-        <c:axId val="572685488"/>
+        <c:axId val="489578216"/>
+        <c:axId val="489582136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="572682744"/>
+        <c:axId val="489578216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -638,7 +677,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572685488"/>
+        <c:crossAx val="489582136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,7 +685,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572685488"/>
+        <c:axId val="489582136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -697,7 +736,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572682744"/>
+        <c:crossAx val="489578216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1452,11 +1491,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="572680392"/>
-        <c:axId val="572680784"/>
+        <c:axId val="489571552"/>
+        <c:axId val="489578608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="572680392"/>
+        <c:axId val="489571552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572680784"/>
+        <c:crossAx val="489578608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="572680784"/>
+        <c:axId val="489578608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="572680392"/>
+        <c:crossAx val="489571552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1723,7 +1762,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Occurences</c:v>
+                  <c:v>Response Occurences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2049,6 +2088,9 @@
                 <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
@@ -2057,6 +2099,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2071,7 +2116,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absent in the Proposal</c:v>
+                  <c:v>Category Present in the Proposal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2374,8 +2419,38 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -2564,7 +2639,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Occurences</c:v>
+                  <c:v>Response Occurences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2629,11 +2704,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'PARKS (Proposal)'!$C$3</c:f>
+              <c:f>'PARKS (Proposal)'!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Absent in the Proposal/ Uncategorized</c:v>
+                  <c:v>Uncategorized Responses</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2673,7 +2748,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARKS (Proposal)'!$C$4:$C$8</c:f>
+              <c:f>'PARKS (Proposal)'!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2693,11 +2768,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="494548520"/>
-        <c:axId val="494554792"/>
+        <c:axId val="489581744"/>
+        <c:axId val="489571160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494548520"/>
+        <c:axId val="489581744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2740,7 +2815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494554792"/>
+        <c:crossAx val="489571160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2748,7 +2823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494554792"/>
+        <c:axId val="489571160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2799,7 +2874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494548520"/>
+        <c:crossAx val="489581744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2983,7 +3058,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'PARKS (Proposal)'!$D$3</c:f>
+              <c:f>'PARKS (Proposal)'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2994,12 +3069,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARKS (Proposal)'!$D$4</c:f>
+              <c:f>'PARKS (Proposal)'!$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.20574162679425836</c:v>
+                  <c:v>0.20673076923076922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3031,7 +3106,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'PARKS (Proposal)'!$D$3</c:f>
+              <c:f>'PARKS (Proposal)'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3042,12 +3117,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARKS (Proposal)'!$D$5</c:f>
+              <c:f>'PARKS (Proposal)'!$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.784688995215311E-2</c:v>
+                  <c:v>4.807692307692308E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3079,7 +3154,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'PARKS (Proposal)'!$D$3</c:f>
+              <c:f>'PARKS (Proposal)'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3090,12 +3165,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARKS (Proposal)'!$D$6</c:f>
+              <c:f>'PARKS (Proposal)'!$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.10576923076923077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3127,7 +3202,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'PARKS (Proposal)'!$D$3</c:f>
+              <c:f>'PARKS (Proposal)'!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3138,12 +3213,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARKS (Proposal)'!$D$7</c:f>
+              <c:f>'PARKS (Proposal)'!$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.3923444976076555E-2</c:v>
+                  <c:v>2.403846153846154E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3158,11 +3233,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="494548912"/>
-        <c:axId val="494555184"/>
+        <c:axId val="489579784"/>
+        <c:axId val="489573512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494548912"/>
+        <c:axId val="489579784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3205,7 +3280,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494555184"/>
+        <c:crossAx val="489573512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3213,7 +3288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494555184"/>
+        <c:axId val="489573512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3264,7 +3339,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494548912"/>
+        <c:crossAx val="489579784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3429,7 +3504,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Occurences</c:v>
+                  <c:v>Response Occurences</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6986,13 +7061,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7018,13 +7093,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>83</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7050,13 +7125,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>716280</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>107</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -7089,7 +7164,7 @@
       <xdr:rowOff>148590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
@@ -7121,7 +7196,7 @@
       <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
@@ -7153,7 +7228,7 @@
       <xdr:rowOff>140970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
       <xdr:row>103</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
@@ -7441,32 +7516,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E17"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H94" sqref="H94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>14</v>
@@ -7479,8 +7554,11 @@
       <c r="B3">
         <v>56</v>
       </c>
+      <c r="C3" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E3">
-        <f>B3/552</f>
+        <f t="shared" ref="E3:E9" si="0">B3/552</f>
         <v>0.10144927536231885</v>
       </c>
     </row>
@@ -7491,8 +7569,11 @@
       <c r="B4">
         <v>19</v>
       </c>
+      <c r="C4" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E4">
-        <f>B4/552</f>
+        <f t="shared" si="0"/>
         <v>3.4420289855072464E-2</v>
       </c>
     </row>
@@ -7503,8 +7584,11 @@
       <c r="B5">
         <v>12</v>
       </c>
+      <c r="C5" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E5">
-        <f>B5/552</f>
+        <f t="shared" si="0"/>
         <v>2.1739130434782608E-2</v>
       </c>
     </row>
@@ -7515,8 +7599,11 @@
       <c r="B6">
         <v>23</v>
       </c>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E6">
-        <f>B6/552</f>
+        <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
@@ -7527,8 +7614,11 @@
       <c r="B7">
         <v>13</v>
       </c>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E7">
-        <f>B7/552</f>
+        <f t="shared" si="0"/>
         <v>2.355072463768116E-2</v>
       </c>
     </row>
@@ -7539,8 +7629,11 @@
       <c r="B8">
         <v>10</v>
       </c>
+      <c r="C8" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E8">
-        <f>B8/552</f>
+        <f t="shared" si="0"/>
         <v>1.8115942028985508E-2</v>
       </c>
     </row>
@@ -7551,8 +7644,11 @@
       <c r="B9">
         <v>6</v>
       </c>
+      <c r="C9" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E9">
-        <f>B9/552</f>
+        <f t="shared" si="0"/>
         <v>1.0869565217391304E-2</v>
       </c>
     </row>
@@ -7560,7 +7656,10 @@
       <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E10">
@@ -7575,6 +7674,9 @@
       <c r="B11">
         <v>9</v>
       </c>
+      <c r="C11" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E11">
         <f>B11/552</f>
         <v>1.6304347826086956E-2</v>
@@ -7587,6 +7689,9 @@
       <c r="B12">
         <v>9</v>
       </c>
+      <c r="C12" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E12">
         <f>B12/552</f>
         <v>1.6304347826086956E-2</v>
@@ -7599,6 +7704,9 @@
       <c r="B13">
         <v>36</v>
       </c>
+      <c r="C13" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="E13">
         <f>B13/552</f>
         <v>6.5217391304347824E-2</v>
@@ -7608,7 +7716,10 @@
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C14">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E14">
@@ -7630,123 +7741,151 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B17">
+        <f>SUM(B3:B14)</f>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
         <f>((552-354)/552)</f>
         <v>0.35869565217391303</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D12"/>
+  <dimension ref="A3:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="62.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>43</v>
       </c>
-      <c r="D4">
-        <f>(B4/209)</f>
-        <v>0.20574162679425836</v>
+      <c r="C4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>(B4/208)</f>
+        <v>0.20673076923076922</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-      <c r="D5">
-        <f>(B5/209)</f>
-        <v>4.784688995215311E-2</v>
+      <c r="C5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>(B5/208)</f>
+        <v>4.807692307692308E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
-      <c r="D6">
-        <f>(B6/209)</f>
-        <v>0.10526315789473684</v>
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>(B6/208)</f>
+        <v>0.10576923076923077</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <f>(B7/209)</f>
-        <v>2.3923444976076555E-2</v>
+      <c r="C7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>(B7/208)</f>
+        <v>2.403846153846154E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8">
         <v>128</v>
       </c>
+      <c r="E8">
+        <f>(D8/208)</f>
+        <v>0.61538461538461542</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <f>SUM(B4:B7)</f>
         <v>80</v>
       </c>
-      <c r="C10">
-        <v>128</v>
-      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <f>((208-128)/208)</f>
+        <v>0.38461538461538464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>